<commit_message>
#32 - CRUD Classes
</commit_message>
<xml_diff>
--- a/public/uploads/StudentsReport.xlsx
+++ b/public/uploads/StudentsReport.xlsx
@@ -1,20 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
-  <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
-  </bookViews>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
+    <sheet sheetId="1" name="Sheet 1" state="visible" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="108">
   <si>
     <t>Name</t>
   </si>
@@ -28,16 +25,88 @@
     <t>Address</t>
   </si>
   <si>
+    <t>user1</t>
+  </si>
+  <si>
+    <t>user1@gmail.com</t>
+  </si>
+  <si>
+    <t>0912345678</t>
+  </si>
+  <si>
+    <t>Viet Nam</t>
+  </si>
+  <si>
+    <t>user2</t>
+  </si>
+  <si>
+    <t>user2@gmail.com</t>
+  </si>
+  <si>
+    <t>user3</t>
+  </si>
+  <si>
+    <t>user3@gmail.com</t>
+  </si>
+  <si>
+    <t>user4</t>
+  </si>
+  <si>
+    <t>user4@gmail.com</t>
+  </si>
+  <si>
+    <t>user5</t>
+  </si>
+  <si>
+    <t>user5@gmail.com</t>
+  </si>
+  <si>
+    <t>user6</t>
+  </si>
+  <si>
+    <t>user6@gmail.com</t>
+  </si>
+  <si>
+    <t>user7</t>
+  </si>
+  <si>
+    <t>user7@gmail.com</t>
+  </si>
+  <si>
+    <t>user8</t>
+  </si>
+  <si>
+    <t>user8@gmail.com</t>
+  </si>
+  <si>
+    <t>user9</t>
+  </si>
+  <si>
+    <t>user9@gmail.com</t>
+  </si>
+  <si>
+    <t>user10</t>
+  </si>
+  <si>
+    <t>user10@gmail.com</t>
+  </si>
+  <si>
     <t>user11</t>
   </si>
   <si>
     <t>user11@gmail.com</t>
   </si>
   <si>
-    <t>0912345678</t>
-  </si>
-  <si>
-    <t>Viet Nam</t>
+    <t>user12</t>
+  </si>
+  <si>
+    <t>user12@gmail.com</t>
+  </si>
+  <si>
+    <t>user13</t>
+  </si>
+  <si>
+    <t>user13@gmail.com</t>
   </si>
   <si>
     <t>user14</t>
@@ -262,112 +331,10 @@
     <t>user50@gmail.com</t>
   </si>
   <si>
-    <t>asdanodsa</t>
-  </si>
-  <si>
-    <t>askdkadsn@gmail.com</t>
-  </si>
-  <si>
-    <t>0912321442</t>
-  </si>
-  <si>
-    <t>Ha noi</t>
-  </si>
-  <si>
-    <t>user100</t>
-  </si>
-  <si>
-    <t>user100@gmail.com</t>
-  </si>
-  <si>
-    <t>user1014</t>
-  </si>
-  <si>
-    <t>user101@gmail.com</t>
-  </si>
-  <si>
-    <t>user102</t>
-  </si>
-  <si>
-    <t>user102@gmail.com</t>
-  </si>
-  <si>
-    <t>user1034</t>
-  </si>
-  <si>
-    <t>user103@gmail.com</t>
-  </si>
-  <si>
-    <t>0912345679</t>
-  </si>
-  <si>
-    <t>user119</t>
-  </si>
-  <si>
-    <t>user119@gmail.com</t>
-  </si>
-  <si>
-    <t>0912345695</t>
-  </si>
-  <si>
-    <t>user120</t>
-  </si>
-  <si>
-    <t>user120@gmail.com</t>
-  </si>
-  <si>
-    <t>0912345696</t>
-  </si>
-  <si>
-    <t>user124</t>
-  </si>
-  <si>
-    <t>user124@gmail.com</t>
-  </si>
-  <si>
-    <t>0912345700</t>
-  </si>
-  <si>
-    <t>user125</t>
-  </si>
-  <si>
-    <t>user125@gmail.com</t>
-  </si>
-  <si>
-    <t>0912345701</t>
-  </si>
-  <si>
-    <t>user126</t>
-  </si>
-  <si>
-    <t>user126@gmail.com</t>
-  </si>
-  <si>
-    <t>0912345702</t>
-  </si>
-  <si>
-    <t>user127</t>
-  </si>
-  <si>
-    <t>user127@gmail.com</t>
-  </si>
-  <si>
-    <t>0912345703</t>
-  </si>
-  <si>
-    <t>user128</t>
-  </si>
-  <si>
-    <t>user128@gmail.com</t>
-  </si>
-  <si>
-    <t>0912345704</t>
-  </si>
-  <si>
-    <t>user</t>
-  </si>
-  <si>
-    <t>user1244@gmail.com</t>
+    <t>ascjashckjhkj@ganul.com</t>
+  </si>
+  <si>
+    <t>asjkcsahkjcs@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -376,27 +343,28 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <b/>
+      <color rgb="FFFFFFFF"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF008000"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -408,16 +376,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -444,44 +410,44 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="1F497D"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="EEECE1"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4F81BD"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="C0504D"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="9BBB59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="8064A2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="4BACC6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="F79646"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -511,12 +477,12 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -555,154 +521,208 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="35000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
+                <a:tint val="100000"/>
                 <a:shade val="100000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+                <a:tint val="50000"/>
+                <a:shade val="100000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="40000">
               <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
+  <a:objectDefaults>
+    <a:spDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </a:style>
+    </a:spDef>
+    <a:lnDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </a:style>
+    </a:lnDef>
+  </a:objectDefaults>
   <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D52"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="D52" sqref="D52"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
     <col min="2" max="2" width="35" customWidth="1"/>
@@ -710,21 +730,21 @@
     <col min="4" max="4" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -738,7 +758,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -752,7 +772,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -766,7 +786,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -780,7 +800,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -794,7 +814,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -808,7 +828,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -822,7 +842,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -836,7 +856,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -850,7 +870,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>24</v>
       </c>
@@ -864,7 +884,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -878,7 +898,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>28</v>
       </c>
@@ -892,7 +912,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>30</v>
       </c>
@@ -906,7 +926,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>32</v>
       </c>
@@ -920,7 +940,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>34</v>
       </c>
@@ -934,7 +954,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>36</v>
       </c>
@@ -948,7 +968,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>38</v>
       </c>
@@ -962,7 +982,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>40</v>
       </c>
@@ -976,7 +996,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>42</v>
       </c>
@@ -990,7 +1010,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>44</v>
       </c>
@@ -1004,7 +1024,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>46</v>
       </c>
@@ -1018,7 +1038,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>48</v>
       </c>
@@ -1032,7 +1052,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>50</v>
       </c>
@@ -1046,7 +1066,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>52</v>
       </c>
@@ -1060,7 +1080,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>54</v>
       </c>
@@ -1074,7 +1094,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>56</v>
       </c>
@@ -1088,7 +1108,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>58</v>
       </c>
@@ -1102,7 +1122,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>60</v>
       </c>
@@ -1116,7 +1136,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>62</v>
       </c>
@@ -1130,7 +1150,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>64</v>
       </c>
@@ -1144,7 +1164,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>66</v>
       </c>
@@ -1158,7 +1178,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>68</v>
       </c>
@@ -1172,7 +1192,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>70</v>
       </c>
@@ -1186,7 +1206,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>72</v>
       </c>
@@ -1200,7 +1220,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>74</v>
       </c>
@@ -1214,7 +1234,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>76</v>
       </c>
@@ -1228,7 +1248,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>78</v>
       </c>
@@ -1242,7 +1262,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>80</v>
       </c>
@@ -1256,7 +1276,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>82</v>
       </c>
@@ -1264,179 +1284,179 @@
         <v>83</v>
       </c>
       <c r="C40" t="s">
+        <v>6</v>
+      </c>
+      <c r="D40" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>84</v>
       </c>
-      <c r="D40" t="s">
+      <c r="B41" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
+      <c r="C41" t="s">
+        <v>6</v>
+      </c>
+      <c r="D41" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>86</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B42" t="s">
         <v>87</v>
       </c>
-      <c r="C41" t="s">
-        <v>6</v>
-      </c>
-      <c r="D41" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
+      <c r="C42" t="s">
+        <v>6</v>
+      </c>
+      <c r="D42" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>88</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B43" t="s">
         <v>89</v>
       </c>
-      <c r="C42" t="s">
-        <v>6</v>
-      </c>
-      <c r="D42" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
+      <c r="C43" t="s">
+        <v>6</v>
+      </c>
+      <c r="D43" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>90</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B44" t="s">
         <v>91</v>
       </c>
-      <c r="C43" t="s">
-        <v>6</v>
-      </c>
-      <c r="D43" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
+      <c r="C44" t="s">
+        <v>6</v>
+      </c>
+      <c r="D44" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>92</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B45" t="s">
         <v>93</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C45" t="s">
+        <v>6</v>
+      </c>
+      <c r="D45" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>94</v>
       </c>
-      <c r="D44" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
+      <c r="B46" t="s">
         <v>95</v>
       </c>
-      <c r="B45" t="s">
+      <c r="C46" t="s">
+        <v>6</v>
+      </c>
+      <c r="D46" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>96</v>
       </c>
-      <c r="C45" t="s">
+      <c r="B47" t="s">
         <v>97</v>
       </c>
-      <c r="D45" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
+      <c r="C47" t="s">
+        <v>6</v>
+      </c>
+      <c r="D47" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>98</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B48" t="s">
         <v>99</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C48" t="s">
+        <v>6</v>
+      </c>
+      <c r="D48" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>100</v>
       </c>
-      <c r="D46" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
+      <c r="B49" t="s">
         <v>101</v>
       </c>
-      <c r="B47" t="s">
+      <c r="C49" t="s">
+        <v>6</v>
+      </c>
+      <c r="D49" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
         <v>102</v>
       </c>
-      <c r="C47" t="s">
+      <c r="B50" t="s">
         <v>103</v>
       </c>
-      <c r="D47" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
+      <c r="C50" t="s">
+        <v>6</v>
+      </c>
+      <c r="D50" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
         <v>104</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B51" t="s">
         <v>105</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C51" t="s">
+        <v>6</v>
+      </c>
+      <c r="D51" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
         <v>106</v>
       </c>
-      <c r="D48" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
+      <c r="B52" t="s">
         <v>107</v>
       </c>
-      <c r="B49" t="s">
-        <v>108</v>
-      </c>
-      <c r="C49" t="s">
-        <v>109</v>
-      </c>
-      <c r="D49" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
-        <v>110</v>
-      </c>
-      <c r="B50" t="s">
-        <v>111</v>
-      </c>
-      <c r="C50" t="s">
-        <v>112</v>
-      </c>
-      <c r="D50" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
-        <v>113</v>
-      </c>
-      <c r="B51" t="s">
-        <v>114</v>
-      </c>
-      <c r="C51" t="s">
-        <v>115</v>
-      </c>
-      <c r="D51" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
-        <v>116</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>117</v>
+      <c r="C52" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B52" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>
 </file>
</xml_diff>